<commit_message>
add function to get data for api from excel file
</commit_message>
<xml_diff>
--- a/unprocessed_files/Lines.xlsx
+++ b/unprocessed_files/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adko8\OneDrive\Desktop\TARS\unprocessed_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8620E1-1A1A-432D-8D5E-BB830DA77A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021F7737-CA3A-4C48-BDE9-1B5B5B714DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{411462C6-0553-4045-81F6-2A96E886D10C}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>May the Force be with you.</t>
   </si>
   <si>
-    <t>I'll be back.</t>
-  </si>
-  <si>
     <t>t0jbNlBVZ17f02VDIeMI</t>
   </si>
   <si>
@@ -66,6 +63,9 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>Hello Ryan</t>
   </si>
 </sst>
 </file>
@@ -440,7 +440,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -451,16 +451,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -468,10 +468,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -482,13 +482,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add unique mp3 file names and output folder
</commit_message>
<xml_diff>
--- a/unprocessed_files/Lines.xlsx
+++ b/unprocessed_files/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adko8\OneDrive\Desktop\TARS\unprocessed_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021F7737-CA3A-4C48-BDE9-1B5B5B714DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B08F77-D885-4EB0-9B67-4C787616C70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{411462C6-0553-4045-81F6-2A96E886D10C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>May the Force be with you.</t>
   </si>
@@ -66,6 +66,33 @@
   </si>
   <si>
     <t>Hello Ryan</t>
+  </si>
+  <si>
+    <t>LcfcDJNUP1GQjkzn1xUU</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>I'm gonna make him an offer he can't refuse.</t>
+  </si>
+  <si>
+    <t>ODq5zmih8GrVes37Dizd</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>Toto, I've a feeling we're not in Kansas anymore.</t>
+  </si>
+  <si>
+    <t>XB0fDUnXU5powFXDhCwa</t>
+  </si>
+  <si>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>There's no crying in baseball!</t>
   </si>
 </sst>
 </file>
@@ -437,15 +464,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE0B8FF-D7DA-43E3-8589-72A8DE89571B}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -491,6 +518,48 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add folder grouping by voice name
</commit_message>
<xml_diff>
--- a/unprocessed_files/Lines.xlsx
+++ b/unprocessed_files/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adko8\OneDrive\Desktop\TARS\unprocessed_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B08F77-D885-4EB0-9B67-4C787616C70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F742476B-1A1D-482B-B9B5-4E399C8B5F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{411462C6-0553-4045-81F6-2A96E886D10C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>May the Force be with you.</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>There's no crying in baseball!</t>
+  </si>
+  <si>
+    <t>I am serious. And don't call me Shirley.</t>
+  </si>
+  <si>
+    <t>You talking to me?</t>
   </si>
 </sst>
 </file>
@@ -464,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE0B8FF-D7DA-43E3-8589-72A8DE89571B}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -560,7 +566,36 @@
         <v>18</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>